<commit_message>
TC for User reglogin  added
</commit_message>
<xml_diff>
--- a/Test-Cases.xlsx
+++ b/Test-Cases.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="463" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98348490-6BF4-463B-AF5C-D6C8665B96E9}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0EF9FF6-5FC4-4FAE-99C4-FA45AF23FDF9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Test_Cases" sheetId="1" r:id="rId1"/>
     <sheet name="User Registration_TestCases" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Login_TestCases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="203">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -459,9 +459,6 @@
     <t>Verify user is able to complete registration by entering a valid OTP.</t>
   </si>
   <si>
-    <t>OTP Sent</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Enter incorrect OTP |
 Valid phone number |
 OTP sent successfully
@@ -502,6 +499,201 @@
   </si>
   <si>
     <t>OTP expired message displayed</t>
+  </si>
+  <si>
+    <t>1. Click Resend OTP |
+Phone number |
+New OTP sent successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New OTP Sent Successfully </t>
+  </si>
+  <si>
+    <t>TC_LOGIN_01</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-01</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-02</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-03</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-04</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-05</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-06</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-07</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-08</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-09</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-10</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-11</t>
+  </si>
+  <si>
+    <t>FR-LOGIN-12</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_01</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_02</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_03</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_04</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_05</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_06</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_07</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_08</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_09</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_10</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_11</t>
+  </si>
+  <si>
+    <t>TS_LOGIN_12</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and valid password</t>
+  </si>
+  <si>
+    <t>Verify login with valid email and invalid password</t>
+  </si>
+  <si>
+    <t>Verify login with invalid email and valid password</t>
+  </si>
+  <si>
+    <t>Verify login with invalid email and invalid password</t>
+  </si>
+  <si>
+    <t>Verify login with empty email and password fields</t>
+  </si>
+  <si>
+    <t>Verify error message for incorrect login credentials</t>
+  </si>
+  <si>
+    <t>Verify password field is masked</t>
+  </si>
+  <si>
+    <t>Verify login button functionality</t>
+  </si>
+  <si>
+    <t>Verify “Forgot Password” link functionality</t>
+  </si>
+  <si>
+    <t>Verify user is redirected to login page when accessing protected pages</t>
+  </si>
+  <si>
+    <t>Verify user can logout successfully</t>
+  </si>
+  <si>
+    <t>Verify session timeout after inactivity</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_02</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_03</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_04</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_05</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_06</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_07</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_08</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_09</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_10</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_11</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_12</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>User account exists with valid email and password</t>
+  </si>
+  <si>
+    <t>1.Enter valid email.
+2.Enter valid passowrd.
+3.Click on login</t>
+  </si>
+  <si>
+    <t>1.Enter invalid email.
+2.Enter invalid passowrd.
+3.Click on login</t>
+  </si>
+  <si>
+    <t>1.Enter valid email.
+2.Enter invalid passowrd.
+3.Click on login</t>
+  </si>
+  <si>
+    <t>1.Enter invalid email.
+2.Enter valid passowrd.
+3.Click on login</t>
+  </si>
+  <si>
+    <t>1.Blank email
+2.Blank Password
+3.Click on login</t>
+  </si>
+  <si>
+    <t>Login page is open</t>
+  </si>
+  <si>
+    <t>1.Enter invalid email
+2.Enter valid password
+3.click login</t>
+  </si>
+  <si>
+    <t>1.Enter Email.
+2.Enter Password</t>
   </si>
 </sst>
 </file>
@@ -572,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -591,6 +783,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -629,11 +824,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1228,98 +1429,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4571448-FDFE-4F01-A516-0ABB06952D87}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="9" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="75.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="36" style="8" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="75.7109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="36" style="9" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" style="14" customWidth="1"/>
     <col min="8" max="8" width="40.140625" customWidth="1"/>
     <col min="9" max="9" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="17" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1327,19 +1528,19 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>64</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1361,155 +1562,155 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1517,19 +1718,19 @@
       <c r="A8" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E8" t="s">
         <v>90</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>91</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1555,19 +1756,19 @@
       <c r="A9" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1584,25 +1785,25 @@
       <c r="A10" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="8">
         <v>1234</v>
       </c>
       <c r="I10" t="s">
@@ -1613,19 +1814,19 @@
       <c r="A11" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>64</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1636,80 +1837,95 @@
       <c r="A12" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="22" t="s">
         <v>130</v>
       </c>
       <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>102</v>
       </c>
       <c r="D13" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="F14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H13" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="C14" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="H14" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E15" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="I14" s="11" t="s">
+      <c r="F15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>139</v>
+      <c r="I15" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1724,13 +1940,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F819213-0935-4CCE-97BE-DCD2DE2E7E49}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G31" sqref="G30:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
@@ -1757,17 +1986,17 @@
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="E8" s="6"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="E9" s="6"/>
       <c r="F9" s="2"/>
     </row>
@@ -1813,59 +2042,341 @@
       <c r="E16" s="6"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="2"/>
       <c r="E17" s="6"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="2"/>
       <c r="E18" s="6"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="2"/>
       <c r="E19" s="6"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="2"/>
+    <row r="21" spans="1:12" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" t="s">
+        <v>194</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>195</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>197</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" t="s">
+        <v>200</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
+        <v>200</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>201</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" t="s">
+        <v>200</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C32" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>